<commit_message>
set corrent path and delate photos
s
</commit_message>
<xml_diff>
--- a/LAB2/LAB2_Zestawienie.xlsx
+++ b/LAB2/LAB2_Zestawienie.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Desktop\git\NAI\LAB2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Desktop\NAI\LAB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5372D5-3A07-47DE-8E0D-6B74F6A27E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3FFA61BC-6C8F-4630-A94F-AC5A5D2358AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -299,6 +299,11 @@
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,11 +313,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
@@ -419,9 +419,19 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8386871103005532E-2"/>
+          <c:y val="0.13818181818181818"/>
+          <c:w val="0.92161312889699443"/>
+          <c:h val="0.67156957960107566"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -442,7 +452,7 @@
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
@@ -472,10 +482,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1.0092413046000002</c:v>
+                  <c:v>4.3477819139999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78432969389999962</c:v>
+                  <c:v>1.1184570730500002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
                   <c:v>5.9940714500000003E-5</c:v>
@@ -483,7 +493,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-54A1-441C-A616-BEE2BE39E8D0}"/>
             </c:ext>
@@ -507,7 +517,7 @@
             <a:solidFill>
               <a:schemeClr val="accent2"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
@@ -548,7 +558,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-54A1-441C-A616-BEE2BE39E8D0}"/>
             </c:ext>
@@ -563,17 +573,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="996974160"/>
-        <c:axId val="996972496"/>
+        <c:axId val="372520808"/>
+        <c:axId val="335468520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="996974160"/>
+        <c:axId val="372520808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -611,7 +620,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="996972496"/>
+        <c:crossAx val="335468520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -619,12 +628,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="996972496"/>
+        <c:axId val="335468520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -670,13 +679,13 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="996974160"/>
+        <c:crossAx val="372520808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -684,6 +693,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,14 +725,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1305,13 +1315,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
+      <xdr:colOff>457201</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -1320,7 +1330,7 @@
         <xdr:cNvPr id="2" name="Wykres 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D9523C4-8529-E55B-8071-7333925152FA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D9523C4-8529-E55B-8071-7333925152FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1342,12 +1352,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EADD4843-FAA4-4D1B-9D18-3C34EE17251A}" name="Tabela1" displayName="Tabela1" ref="Q2:S5" totalsRowShown="0">
-  <autoFilter ref="Q2:S5" xr:uid="{EADD4843-FAA4-4D1B-9D18-3C34EE17251A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="Q2:S5" totalsRowShown="0">
+  <autoFilter ref="Q2:S5"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00D72822-0CE1-4991-A5DC-F646F6B0AC79}" name="Kolumna1"/>
-    <tableColumn id="2" xr3:uid="{5594EF0D-994F-4C7D-AD4C-5E567EBE7620}" name="Avg result"/>
-    <tableColumn id="3" xr3:uid="{D3A74A79-4C87-4FA9-A6B7-29AF415E0EB1}" name="Avg Time"/>
+    <tableColumn id="1" name="Kolumna1"/>
+    <tableColumn id="2" name="Avg result"/>
+    <tableColumn id="3" name="Avg Time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1649,16 +1659,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A015AF7-58F8-46CA-8C9D-38C85E25AD69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
@@ -1669,24 +1694,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="G2" s="12" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="L2" s="13" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="L2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
       <c r="Q2" t="s">
         <v>51</v>
       </c>
@@ -1739,7 +1764,7 @@
       </c>
       <c r="R3">
         <f>SUM(D4:D23)/20</f>
-        <v>1.0092413046000002</v>
+        <v>4.3477819139999999E-2</v>
       </c>
       <c r="S3">
         <f>(SUM(E4:E23)/20)/1000000</f>
@@ -1747,10 +1772,10 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>3.5832999999999999</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>1.6406700000000001</v>
       </c>
       <c r="D4" s="5">
@@ -1765,7 +1790,7 @@
       <c r="H4" s="4">
         <v>2.9913400000000001</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="15">
         <v>2.5889899999999999E-4</v>
       </c>
       <c r="J4" s="6">
@@ -1788,7 +1813,7 @@
       </c>
       <c r="R4" s="10">
         <f>SUM(I4:I23)/20</f>
-        <v>0.78432969389999962</v>
+        <v>1.1184570730500002E-2</v>
       </c>
       <c r="S4">
         <f>(SUM(J4:J23)/20)/1000000</f>
@@ -1796,10 +1821,10 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>3.5872799999999998</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>-1.85209</v>
       </c>
       <c r="D5" s="5">
@@ -1814,7 +1839,7 @@
       <c r="H5" s="3">
         <v>-3.0013700000000001</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="15">
         <v>3.3405400000000002E-4</v>
       </c>
       <c r="J5" s="6">
@@ -1845,14 +1870,14 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>3.0009000000000001</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>2.00034</v>
       </c>
       <c r="D6" s="5">
-        <v>3.79312</v>
+        <v>3.7931200000000001E-3</v>
       </c>
       <c r="E6" s="6">
         <v>554250</v>
@@ -1863,7 +1888,7 @@
       <c r="H6" s="4">
         <v>2.9812699999999999</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="15">
         <v>6.3377799999999999E-4</v>
       </c>
       <c r="J6" s="6">
@@ -1883,10 +1908,10 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>-3.78098</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>-3.2834500000000002</v>
       </c>
       <c r="D7" s="5">
@@ -1901,8 +1926,8 @@
       <c r="H7" s="4">
         <v>3.00569</v>
       </c>
-      <c r="I7" s="18">
-        <v>6.7795500000000004</v>
+      <c r="I7" s="15">
+        <v>6.7795500000000002E-6</v>
       </c>
       <c r="J7" s="6">
         <v>392395</v>
@@ -1921,10 +1946,10 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>-3.5849099999999998</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>-1.83992</v>
       </c>
       <c r="D8" s="5">
@@ -1939,8 +1964,8 @@
       <c r="H8" s="4">
         <v>3.0050599999999998</v>
       </c>
-      <c r="I8" s="18">
-        <v>5.60426</v>
+      <c r="I8" s="15">
+        <v>5.6042599999999996E-6</v>
       </c>
       <c r="J8" s="6">
         <v>388605</v>
@@ -1959,10 +1984,10 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>3.0004200000000001</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="11">
         <v>1.9953099999999999</v>
       </c>
       <c r="D9" s="5">
@@ -1977,7 +2002,7 @@
       <c r="H9" s="4">
         <v>2.9933200000000002</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="15">
         <v>1.91387E-4</v>
       </c>
       <c r="J9" s="6">
@@ -1997,10 +2022,10 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>3.5831599999999999</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="11">
         <v>-1.84216</v>
       </c>
       <c r="D10" s="5">
@@ -2015,8 +2040,8 @@
       <c r="H10" s="4">
         <v>2.9982600000000001</v>
       </c>
-      <c r="I10" s="18">
-        <v>2.1403400000000001</v>
+      <c r="I10" s="15">
+        <v>0.214034</v>
       </c>
       <c r="J10" s="6">
         <v>388305</v>
@@ -2035,10 +2060,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>2.9988700000000001</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="11">
         <v>2.0031699999999999</v>
       </c>
       <c r="D11" s="5">
@@ -2053,7 +2078,7 @@
       <c r="H11" s="4">
         <v>2.9905300000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="15">
         <v>3.0957400000000001E-4</v>
       </c>
       <c r="J11" s="6">
@@ -2073,14 +2098,14 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>-3.7786</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="11">
         <v>-3.2825600000000001</v>
       </c>
       <c r="D12" s="5">
-        <v>3.4314</v>
+        <v>3.4313999999999999E-6</v>
       </c>
       <c r="E12" s="6">
         <v>552421</v>
@@ -2091,7 +2116,7 @@
       <c r="H12" s="4">
         <v>3.0053299999999998</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="15">
         <v>3.7429299999999999E-4</v>
       </c>
       <c r="J12" s="6">
@@ -2111,14 +2136,14 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>-3.5852300000000001</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="5">
-        <v>5.7941000000000003</v>
+        <v>0.57940999999999998</v>
       </c>
       <c r="E13" s="6">
         <v>564504</v>
@@ -2129,8 +2154,8 @@
       <c r="H13" s="4">
         <v>2.99831</v>
       </c>
-      <c r="I13" s="18">
-        <v>1.1528</v>
+      <c r="I13" s="15">
+        <v>1.1528E-6</v>
       </c>
       <c r="J13" s="6">
         <v>389321</v>
@@ -2149,10 +2174,10 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>3.5834800000000002</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="11">
         <v>-1.8499399999999999</v>
       </c>
       <c r="D14" s="5">
@@ -2167,7 +2192,7 @@
       <c r="H14" s="4">
         <v>3.00529</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="15">
         <v>3.3111499999999999E-4</v>
       </c>
       <c r="J14" s="6">
@@ -2187,10 +2212,10 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <v>3.0019399999999998</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>1.9998100000000001</v>
       </c>
       <c r="D15" s="5">
@@ -2205,7 +2230,7 @@
       <c r="H15" s="4">
         <v>3.0268000000000002</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="15">
         <v>1.3247599999999999E-3</v>
       </c>
       <c r="J15" s="6">
@@ -2225,10 +2250,10 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <v>-2.80626</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="11">
         <v>3.1278899999999998</v>
       </c>
       <c r="D16" s="5">
@@ -2243,7 +2268,7 @@
       <c r="H16" s="4">
         <v>3.0095200000000002</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="15">
         <v>1.27144E-3</v>
       </c>
       <c r="J16" s="6">
@@ -2263,10 +2288,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <v>-3.7797399999999999</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="11">
         <v>-3.2802899999999999</v>
       </c>
       <c r="D17" s="5">
@@ -2281,7 +2306,7 @@
       <c r="H17" s="4">
         <v>2.9945400000000002</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <v>5.1033100000000004E-4</v>
       </c>
       <c r="J17" s="6">
@@ -2301,10 +2326,10 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <v>3.5810300000000002</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="11">
         <v>-1.8489500000000001</v>
       </c>
       <c r="D18" s="5">
@@ -2319,7 +2344,7 @@
       <c r="H18" s="4">
         <v>2.9986299999999999</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="15">
         <v>2.5045299999999998E-4</v>
       </c>
       <c r="J18" s="6">
@@ -2339,14 +2364,14 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <v>3.5839500000000002</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <v>-1.8465400000000001</v>
       </c>
-      <c r="D19" s="17">
-        <v>4.3539399999999997</v>
+      <c r="D19" s="14">
+        <v>4.3539399999999999E-5</v>
       </c>
       <c r="E19" s="6">
         <v>555964</v>
@@ -2357,7 +2382,7 @@
       <c r="H19" s="4">
         <v>3.02847</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="15">
         <v>2.0725100000000001E-3</v>
       </c>
       <c r="J19" s="6">
@@ -2377,14 +2402,14 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <v>-2.8060399999999999</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="11">
         <v>3.1313900000000001</v>
       </c>
       <c r="D20" s="5">
-        <v>2.806622</v>
+        <v>0.28066219999999997</v>
       </c>
       <c r="E20" s="6">
         <v>552297</v>
@@ -2395,7 +2420,7 @@
       <c r="H20" s="4">
         <v>3.0093399999999999</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="15">
         <v>1.5728300000000001E-4</v>
       </c>
       <c r="J20" s="6">
@@ -2415,10 +2440,10 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="15">
+      <c r="B21" s="12">
         <v>3.0002900000000001</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="11">
         <v>2.0045700000000002</v>
       </c>
       <c r="D21" s="5">
@@ -2433,7 +2458,7 @@
       <c r="H21" s="4">
         <v>2.98712</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="15">
         <v>3.4023099999999998E-4</v>
       </c>
       <c r="J21" s="6">
@@ -2453,10 +2478,10 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="15">
+      <c r="B22" s="12">
         <v>2.8043499999999999</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="11">
         <v>3.1327799999999999</v>
       </c>
       <c r="D22" s="5">
@@ -2471,7 +2496,7 @@
       <c r="H22" s="4">
         <v>3.0216599999999998</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="15">
         <v>8.7721999999999995E-4</v>
       </c>
       <c r="J22" s="6">
@@ -2491,10 +2516,10 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>-2.9975100000000001</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="11">
         <v>1.9979499999999999</v>
       </c>
       <c r="D23" s="5">
@@ -2509,7 +2534,7 @@
       <c r="H23" s="4">
         <v>3.0063200000000001</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="15">
         <v>4.0654999999999999E-4</v>
       </c>
       <c r="J23" s="6">
@@ -2535,7 +2560,7 @@
       <c r="E24" s="6"/>
       <c r="G24" s="2"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="6"/>
       <c r="L24" s="2"/>
       <c r="M24" s="4"/>

</xml_diff>